<commit_message>
Finish TF-IDF & EDA
</commit_message>
<xml_diff>
--- a/textToOps/data/processed/prediction_vs_actual.xlsx
+++ b/textToOps/data/processed/prediction_vs_actual.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,31 +462,31 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>What are the four fire stations with shortest network-based paths to 1202 Twin Peaks Blvd in San Francisco</t>
+          <t>What are the areas within a four-minute drive of each fire station at 2 a.m. on Tuesday in Utrecht</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>what be the unitN fire station with shortest unitN path to unitN twin peak blvd in san francisco</t>
+          <t>what be the area within a unitT drive of each fire station at unitN unitTR on dayofaweek in utrecht</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="F2" t="n">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>135</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -510,64 +510,64 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>What areas are not flood plain in Houston</t>
+          <t>What are the land use inside the flood zones in Oleander</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>what area be not flood plain in houston</t>
+          <t>what be the land use inside the flood unitN in oleander</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>137</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tell me not flood plain area in Houston</t>
+          <t>What area are within 50 km from family physician services in Saskatchewan in Canada</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>tell me not flood plain area in houston</t>
+          <t>what area be within unitN unitL from family physician service in saskatchewan in canada</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>138</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>What areas are outside 155 meters from nature reserve districts in Houston</t>
+          <t>What areas are at least 3000 meters from the rivers in Spain</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>what area be outside unitN unitL from nature reserve district in houston</t>
+          <t>what area be at least unitN unitL from the river in spain</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -582,16 +582,16 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>139</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>What areas are outside 3000 meters of the rivers in Spain</t>
+          <t>What areas are inside 1000 foot of schools in El Cajon</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>what area be outside unitN unitL of the river in spain</t>
+          <t>what area be inside unitN unitL of school in el cajon</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -606,16 +606,16 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>140</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>What areas are outside 5000 meters of the roads in Spain</t>
+          <t>What areas are more than 5000 meters from the roads in Spain</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>what area be outside unitN unitL of the road in spain</t>
+          <t>what area be more than unitN unitL from the road in spain</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -630,136 +630,136 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>141</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>What areas are within 1000 meters of the major transport routes in Amsterdam</t>
+          <t>What areas are green belt areas in Houston</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>what area be within unitN unitL of the major transport route in amsterdam</t>
+          <t>what area be green belt area in houston</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>142</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>What areas are reachable within 3 minutes of by car from the nearest fire station (from my current location) in Oleander</t>
+          <t>What areas are not classified as flood plain in Houston</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>what area be reachable within unitN unitT of by car from the near fire station from my current location in oleander</t>
+          <t>what area be not classify a flood plain in houston</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="E10" t="n">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
-        <v>53</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>What areas are outside 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
+          <t>Tell me not flood plain area in Houston</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>what area be outside unitN unitT of drive time from the near fire station from my current location in oleander</t>
+          <t>tell me not flood plain area in houston</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="E11" t="n">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
-        <v>53</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>144</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>What areas are within 500 meters from religious places in Karbala in Iraq</t>
+          <t>What areas are not park in Houston</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>what area be within unitN unitL from religious place in karbala in iraq</t>
+          <t>what area be not park in houston</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>145</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>What areas are within 500 meters from universities in Karbala in Iraq</t>
+          <t>What areas are not wetlands in Houston</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>what area be within unitN unitL from university in karbala in iraq</t>
+          <t>what area be not wetland in houston</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>146</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>What areas are within a quarter mile of a restaurant in Gresham</t>
+          <t>What areas are outside 150 meters from schools in Houston</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>what area be within a quarter mile of a restaurant in gresham</t>
+          <t>what area be outside unitN unitL from school in houston</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -769,21 +769,21 @@
         <v>8</v>
       </c>
       <c r="F14" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>What areas are within a quarter mile of a store in Gresham</t>
+          <t>What areas are outside 5000 meters of the roads in Spain</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>what area be within a quarter mile of a store in gresham</t>
+          <t>what area be outside unitN unitL of the road in spain</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -793,21 +793,21 @@
         <v>8</v>
       </c>
       <c r="F15" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>What areas are within a quarter mile of light rail stop in Gresham</t>
+          <t>What areas are outside 60 meters from water body in Houston</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>what area be within a quarter mile of light rail stop in gresham</t>
+          <t>what area be outside unitN unitL from water body in houston</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -817,549 +817,549 @@
         <v>8</v>
       </c>
       <c r="F16" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>149</v>
+        <v>15</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>What areas are accessible within two miles of urban landuse in Loudoun County in US</t>
+          <t>What areas are within 1000 meters of roads in Assam in India</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>what area be accessible within unitN mile of urban landuse in loudoun county in u</t>
+          <t>what area be within unitN unitL of road in assam in india</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E17" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>150</v>
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>What areas do have temperature in Celsius less than 0 degrees in Spain</t>
+          <t>What areas are within 1000 meters of the schools in Oleander</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>what area do have temperature in celsius less than unitN degree in spain</t>
+          <t>what area be within unitN unitL of the school in oleander</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="E18" t="n">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>What areas have an monthly rainfall of more than 1000 millimeters in the Cape Peninsula</t>
+          <t>What areas are accessible within 3 minutes of by car from the nearest fire station (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>what area have an monthly rainfall of more than unitN unitL in the cape peninsula</t>
+          <t>what area be accessible within unitN unitT of by car from the near fire station from my current location in oleander</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E19" t="n">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F19" t="n">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>152</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>What areas have slope larger than 15 percent and smaller than 60 percent in the Cape Peninsula</t>
+          <t>What areas are within 3 minutes of by car from the nearest fire station (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>what area have slope large than unitN percent and small than unitN percent in the cape peninsula</t>
+          <t>what area be within unitN unitT of by car from the near fire station from my current location in oleander</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E20" t="n">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F20" t="n">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>153</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>What houses are for sale and within 0.5km from the main roads in Utrecht</t>
+          <t>What areas are outside 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>what house be for sale and within unitL from the main road in utrecht</t>
+          <t>what area be outside unitN unitT of drive time from the near fire station from my current location in oleander</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="E21" t="n">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="F21" t="n">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Which houses are larger than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
+          <t>What areas are within 300 meters of runways in Schiphol airport</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>which house be large than unitN square unitL and within unitL from the near school from my current location in utrecht</t>
+          <t>what area be within unitN unitL of runway in schiphol airport</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E22" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>155</v>
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>What houses are less than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
+          <t>What areas are within 60 minutes of airports in Crook, Deschutes, and Jefferson county</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>what house be less than unitN square unitL and within unitL from the near school from my current location in utrecht</t>
+          <t>what area be within unitN unitT of airport in crook deschutes and jefferson county</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E23" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F23" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>156</v>
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>What houses are for sale in flood zone in Utrecht</t>
+          <t>What areas are within 800 meter from major highways in Houston</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>what house be for sale in flood unitN in utrecht</t>
+          <t>what area be within unitN unitL from major highway in houston</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E24" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>157</v>
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>What houses are for sale in urban areas in Utrecht</t>
+          <t>What areas are within a quarter mile of a restaurant in Gresham</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>what house be for sale in urban area in utrecht</t>
+          <t>what area be within a quarter mile of a restaurant in gresham</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E25" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>158</v>
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>What is the average rating of street pavement for each borough in New York City</t>
+          <t>What areas are within a quarter mile of a store in Gresham</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>what be the average rating of street pavement for each borough in new york city</t>
+          <t>what area be within a quarter mile of a store in gresham</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E26" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Show me the central feature of bank branches in Oleander</t>
+          <t>What areas are within a quarter mile of light rail stop in Gresham</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>show me the central feature of bank branch in oleander</t>
+          <t>what area be within a quarter mile of light rail stop in gresham</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E27" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F27" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>160</v>
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>What is weighted average coordinates of bank branches in Oleander</t>
+          <t>What areas are accessible within reach two miles of urban landuse in Loudoun County in US</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>what be unitN average coordinate of bank branch in oleander</t>
+          <t>what area be accessible within reach unitN mile of urban landuse in loudoun county in u</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E28" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F28" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>161</v>
+        <v>27</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to the rivers in Crook, Deschutes, and Jefferson county</t>
+          <t>What areas are accessible within two miles of urban landuse in Loudoun County in US</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>what be the euclidean distance to the river in crook deschutes and jefferson county</t>
+          <t>what area be accessible within unitN mile of urban landuse in loudoun county in u</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F29" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>162</v>
+        <v>28</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to tram stations in Amsterdam</t>
+          <t>What areas have an annual rainfall of less than 1000 millimeters in the Cape Peninsula</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>what be the euclidean distance to tram station in amsterdam</t>
+          <t>what area have an annual rainfall of less than unitN unitL in the cape peninsula</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="F30" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>What is the interpolated surface of ozone concentration in California</t>
+          <t>What areas have an monthly rainfall of more than 1000 millimeters in the Cape Peninsula</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>what be the interpolate surface of unitN concentration in california</t>
+          <t>what area have an monthly rainfall of more than unitN unitL in the cape peninsula</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="E31" t="n">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F31" t="n">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>What is the kernel density of traffic accidents in Pasadena, California</t>
+          <t>What areas have an annual rainfall of more than 1000 millimeters in the Cape Peninsula</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>what be the kernel density of traffic accident in pasadena california</t>
+          <t>what area have an annual rainfall of more than unitN unitL in the cape peninsula</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="F32" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>165</v>
+        <v>31</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>What is the land use in Netherlands</t>
+          <t>What areas have an aspect larger than 45 degree and smaller than 135 degrees in the Cape Peninsula</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>what be the land use in netherlands</t>
+          <t>what area have an aspect large than unitN degree and small than unitN degree in the cape peninsula</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="F33" t="n">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>What is the literacy rate for each country in Africa</t>
+          <t>What areas have slope larger than 15 percent and smaller than 60 percent in the Cape Peninsula</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>what be the literacy rate for each country in africa</t>
+          <t>what area have slope large than unitN percent and small than unitN percent in the cape peninsula</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="F34" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>167</v>
+        <v>33</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>What is the mean center of crimes weighted by the severity in Fort Worth</t>
+          <t>What houses are larger than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>what be the mean center of crime unitN by the severity in fort worth</t>
+          <t>what house be large than unitN square unitL and within unitL from the near school from my current location in utrecht</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="F35" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>168</v>
+        <v>34</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>What is the mean center of the fire calls for each alarm territory in Fort Worth in 2017</t>
+          <t>What houses are for sale and within 1km from the nearest subway station (from my current location) in Utrecht</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>what be the mean center of the fire call for each alarm territory in fort worth in unitN</t>
+          <t>what house be for sale and within unitL from the near subway station from my current location in utrecht</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="E36" t="n">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F36" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>169</v>
+        <v>35</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>What is the median population for each census block in Tarrant County in Texas</t>
+          <t>What houses are less than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>what be the median population for each census block in tarrant county in texas</t>
+          <t>what house be less than unitN square unitL and within unitL from the near school from my current location in utrecht</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E37" t="n">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F37" t="n">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>170</v>
+        <v>36</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>What is the number of crime cases for each police district in Texas in 2018</t>
+          <t>What houses are for sale outside flood zone in Utrecht</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>what be the number of crime case for each police district in texas in unitN</t>
+          <t>what house be for sale outside flood unitN in utrecht</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E38" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F38" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>171</v>
+        <v>37</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>What is the number of dwelling units inside the flood zones in Oleander</t>
+          <t>What houses are less than 30 square meters in urban areas in Utrecht</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>what be the number of dwell unit inside the flood unitN in oleander</t>
+          <t>what house be less than unitN square unitL in urban area in utrecht</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1374,112 +1374,112 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>172</v>
+        <v>38</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>What is the number of high school students for each senior high school district in Oleander</t>
+          <t>What is the area of currently mixed use zones in Gresham</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>what be the number of high school student for each senior high school district in oleander</t>
+          <t>what be the area of currently mixed use unitN in gresham</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="E40" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>173</v>
+        <v>39</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>What is the point density of fire calls in Oleander</t>
+          <t>Tell me the central feature of bank branches in Oleander</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>what be the point density of fire call in oleander</t>
+          <t>tell me the central feature of bank branch in oleander</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E41" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F41" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>174</v>
+        <v>40</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>What is the tornado path in Oleander in April 2011</t>
+          <t>Tell me weighted average coordinates of bank branches in Oleander</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>what be the tornado path in oleander in montInYe unitN</t>
+          <t>tell me unitN average coordinate of bank branch in oleander</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F42" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>175</v>
+        <v>41</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>What is the total area of agriculture in Netherlands</t>
+          <t>What is weighted average coordinates of bank branches in Oleander</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>what be the total area of agriculture in netherlands</t>
+          <t>what be unitN average coordinate of bank branch in oleander</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E43" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="F43" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>176</v>
+        <v>42</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>What is the total population for each census block in Tarrant County, Texas</t>
+          <t>What is the cervix cancer mortality rate of white females for each city in the Western USA from 1970 to 1994</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>what be the total population for each census block in tarrant county texas</t>
+          <t>what be the cervix cancer mortality rate of white female for each city in the western usa from unitN to unitN</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1489,196 +1489,196 @@
         <v>2</v>
       </c>
       <c r="F44" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>177</v>
+        <v>43</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>What liquor stores are within 1000 foot of parks in El Cajon</t>
+          <t>What is the density surface of temperature measurements in Oleander city</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>what liquor store be within unitN unitL of park in el cajon</t>
+          <t>what be the density surface of temperature measurement in oleander city</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E45" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>178</v>
+        <v>44</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Where are forestry lands in Happy Valley ski resort</t>
+          <t>What is the Euclidean distance to green areas in Amsterdam</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>where be forestry land in happy valley ski resort</t>
+          <t>what be the euclidean distance to green area in amsterdam</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>179</v>
+        <v>45</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Where are the commercial areas in Amsterdam</t>
+          <t>What is the Euclidean distance to recreational sites in Utrecht</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>where be the commercial area in amsterdam</t>
+          <t>what be the euclidean distance to recreational site in utrecht</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E47" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>180</v>
+        <v>46</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Where are the industrial areas in Utrecht</t>
+          <t>What is the hot spots and cold spots for average loan interest rates in the US</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>where be the industrial area in utrecht</t>
+          <t>what be the hot spot and cold spot for average loan interest rate in the u</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E48" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F48" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>181</v>
+        <v>47</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Where are the luxury hotels with more than 20 bedrooms in Happy Valley ski resort</t>
+          <t>What is the interpolated surface of ozone concentration in California</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>where be the luxury hotel with more than unitN bedroom in happy valley ski resort</t>
+          <t>what be the interpolate surface of unitN concentration in california</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E49" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>182</v>
+        <v>48</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Which houses are within 2 minutes driving time from fire stations  (from my current location) in Oleander</t>
+          <t>What is the kernel density of crime in Surrey in UK</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>which house be within unitN unitT drive time from fire station from my current location in oleander</t>
+          <t>what be the kernel density of crime in surrey in uk</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="E50" t="n">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
-        <v>53</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>183</v>
+        <v>49</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Which houses have construction year between 1990 and 2000 in Utrecht</t>
+          <t>What is the kernel density of traffic accidents in Pasadena, California</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>which house have construction year between unitN and unitN in utrecht</t>
+          <t>what be the kernel density of traffic accident in pasadena california</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>184</v>
+        <v>50</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Which park is biggest in Utrecht</t>
+          <t>What is the land use in the Happy Valley resort</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>which park be big in utrecht</t>
+          <t>what be the land use in the happy valley resort</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -1686,73 +1686,841 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>185</v>
+        <v>51</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Which schools are not accessible within 3 minutes by a car from a fire station in Fort Worth</t>
+          <t>What is the lung cancer mortality rate of white males for each city in the Western USA from 1970 to 1994</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>which school be not accessible within unitN unitT by a car from a fire station in fort worth</t>
+          <t>what be the lung cancer mortality rate of white male for each city in the western usa from unitN to unitN</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E53" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>186</v>
+        <v>52</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Which schools are not within 3 minutes of driving time from a fire station in Fort Worth</t>
+          <t>What is the mean center of crimes weighted by the severity in Fort Worth</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>which school be not within unitN unitT of drive time from a fire station in fort worth</t>
+          <t>what be the mean center of crime unitN by the severity in fort worth</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E54" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>187</v>
+        <v>53</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>What is the mean center of library patrons for each district in Oleander</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>what be the mean center of library patron for each district in oleander</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>16</v>
+      </c>
+      <c r="E55" t="n">
+        <v>16</v>
+      </c>
+      <c r="F55" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>What is the mean center of the fire calls for each alarm territory in Fort Worth in 2017</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>what be the mean center of the fire call for each alarm territory in fort worth in unitN</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>16</v>
+      </c>
+      <c r="E56" t="n">
+        <v>16</v>
+      </c>
+      <c r="F56" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Tell me the median household income for each census block in Tarrant County in Texas</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>tell me the median household income for each census block in tarrant county in texas</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>28</v>
+      </c>
+      <c r="E57" t="n">
+        <v>28</v>
+      </c>
+      <c r="F57" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>What is the median number of family member for each census block in Tarrant County in Texas</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>what be the median number of family member for each census block in tarrant county in texas</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>28</v>
+      </c>
+      <c r="E58" t="n">
+        <v>28</v>
+      </c>
+      <c r="F58" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>What is the median population for each census block in Tarrant County in Texas</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>what be the median population for each census block in tarrant county in texas</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>28</v>
+      </c>
+      <c r="E59" t="n">
+        <v>28</v>
+      </c>
+      <c r="F59" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>What is the median people age for each census tract in Tarrant County in Texas</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>what be the median people age for each census tract in tarrant county in texas</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>28</v>
+      </c>
+      <c r="E60" t="n">
+        <v>28</v>
+      </c>
+      <c r="F60" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>What is the number of election votes for each precinct in Dallas</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>what be the number of election vote for each precinct in dallas</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>27</v>
+      </c>
+      <c r="E61" t="n">
+        <v>27</v>
+      </c>
+      <c r="F61" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>What is the number of high school students for each senior high school district in Oleander</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>what be the number of high school student for each senior high school district in oleander</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>27</v>
+      </c>
+      <c r="E62" t="n">
+        <v>27</v>
+      </c>
+      <c r="F62" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>What is the number of inhabitants for each village in Banten province in Indonesia</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>what be the number of inhabitant for each village in unitN province in unitN</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>27</v>
+      </c>
+      <c r="E63" t="n">
+        <v>27</v>
+      </c>
+      <c r="F63" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>What is the point density of cycling destinations in the Metro Vancouver region in Canada</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>what be the point density of cycling destination in the metro vancouver region in canada</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>32</v>
+      </c>
+      <c r="E64" t="n">
+        <v>32</v>
+      </c>
+      <c r="F64" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>What is the point density of fire calls in Oleander</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>what be the point density of fire call in oleander</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>32</v>
+      </c>
+      <c r="E65" t="n">
+        <v>32</v>
+      </c>
+      <c r="F65" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>What is the population density in California</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>what be the population density in california</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>33</v>
+      </c>
+      <c r="E66" t="n">
+        <v>33</v>
+      </c>
+      <c r="F66" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>What is the total area of agriculture in Netherlands</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>what be the total area of agriculture in netherlands</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>33</v>
+      </c>
+      <c r="E67" t="n">
+        <v>33</v>
+      </c>
+      <c r="F67" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>What is the total population within a four-minute travel time from fire stations in Poway</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>what be the total population within a unitT travel time from fire station in poway</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>50</v>
+      </c>
+      <c r="E68" t="n">
+        <v>50</v>
+      </c>
+      <c r="F68" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>What liquor stores are within 1000 foot of libraries in El Cajon</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>what liquor store be within unitN unitL of library in el cajon</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>21</v>
+      </c>
+      <c r="E69" t="n">
+        <v>21</v>
+      </c>
+      <c r="F69" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>What liquor stores are within 1000 foot of parks in El Cajon</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>what liquor store be within unitN unitL of park in el cajon</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>21</v>
+      </c>
+      <c r="E70" t="n">
+        <v>21</v>
+      </c>
+      <c r="F70" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Where are not conservation areas in UK</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>where be not conservation area in uk</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>18</v>
+      </c>
+      <c r="E71" t="n">
+        <v>18</v>
+      </c>
+      <c r="F71" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Where are not protected region in Assam in India</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>where be not protect region in assam in india</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>18</v>
+      </c>
+      <c r="E72" t="n">
+        <v>18</v>
+      </c>
+      <c r="F72" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Where are the accidents within ski pistes in the Happy Valley</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>where be the accident within ski piste in the happy valley</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>14</v>
+      </c>
+      <c r="E73" t="n">
+        <v>14</v>
+      </c>
+      <c r="F73" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Where are the auto accidents in Tarrant County in Texas</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>where be the auto accident in tarrant county in texas</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>2</v>
+      </c>
+      <c r="E74" t="n">
+        <v>2</v>
+      </c>
+      <c r="F74" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Where are the rocky areas in Spain</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>where be the rocky area in spain</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>18</v>
+      </c>
+      <c r="E75" t="n">
+        <v>18</v>
+      </c>
+      <c r="F75" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Where are the ski pistes in Happy Valley ski resort</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>where be the ski piste in happy valley ski resort</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>18</v>
+      </c>
+      <c r="E76" t="n">
+        <v>18</v>
+      </c>
+      <c r="F76" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Which houses are for sale in Utrecht</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>which house be for sale in utrecht</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>2</v>
+      </c>
+      <c r="E77" t="n">
+        <v>2</v>
+      </c>
+      <c r="F77" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Which houses are within 2 minutes driving time from fire stations  (from my current location) in Oleander</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>which house be within unitN unitT drive time from fire station from my current location in oleander</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>42</v>
+      </c>
+      <c r="E78" t="n">
+        <v>42</v>
+      </c>
+      <c r="F78" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Which land use contains meteorological stations in Netherlands</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>which land use contains meteorological station in netherlands</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>14</v>
+      </c>
+      <c r="E79" t="n">
+        <v>14</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Which park is biggest in Utrecht</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>which park be big in utrecht</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>18</v>
+      </c>
+      <c r="E80" t="n">
+        <v>18</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Which schools are not reachable within 3 minutes of driving time from a fire station in Fort Worth</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>which school be not reachable within unitN unitT of drive time from a fire station in fort worth</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>50</v>
+      </c>
+      <c r="E81" t="n">
+        <v>50</v>
+      </c>
+      <c r="F81" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Which shops are open at 6 pm in Happy Valley ski resort</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>which shop be open at unitN unitTR in happy valley ski resort</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Which vacant lots are within 1 mile of a freeway in Hillsboro</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>which vacant lot be within unitN mile of a freeway in hillsboro</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>21</v>
+      </c>
+      <c r="E83" t="n">
+        <v>21</v>
+      </c>
+      <c r="F83" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Which visitor facilities are in the Happy Valley</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>which visitor facility be in the happy valley</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Which suggested wind farm are nearest to the high way in Scotland</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>which suggest wind farm be near to the high way in scotland</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>13</v>
+      </c>
+      <c r="E85" t="n">
+        <v>13</v>
+      </c>
+      <c r="F85" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
           <t>Which proposed wind farm are nearest to the high way in Scotland</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="C86" t="inlineStr">
         <is>
           <t>which propose wind farm be near to the high way in scotland</t>
         </is>
       </c>
-      <c r="D55" t="n">
+      <c r="D86" t="n">
         <v>13</v>
       </c>
-      <c r="E55" t="n">
+      <c r="E86" t="n">
         <v>13</v>
       </c>
-      <c r="F55" t="n">
+      <c r="F86" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Which wind farm proposals are nearest to the roads in Scotland</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>which wind farm proposal be near to the road in scotland</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>13</v>
+      </c>
+      <c r="E87" t="n">
+        <v>13</v>
+      </c>
+      <c r="F87" t="n">
         <v>13</v>
       </c>
     </row>

</xml_diff>